<commit_message>
renamed model.py to custom_resnet.py
</commit_message>
<xml_diff>
--- a/Observation.xlsx
+++ b/Observation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bala/Desktop/Projects/ERA/Session10/ModularRepository/modular/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B87CBEB6-A55A-B840-9890-C03B45F6F777}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C119AD0-055C-8F4E-BD52-EC83EDFB3C78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{F215A8E2-2D1F-A441-B7FA-652D74289773}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17180" xr2:uid="{F215A8E2-2D1F-A441-B7FA-652D74289773}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -432,8 +432,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14F4F4F4-6DB4-9E47-9C42-B8C813E0545D}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -524,6 +524,12 @@
       <c r="C4">
         <v>50</v>
       </c>
+      <c r="D4">
+        <v>67.64</v>
+      </c>
+      <c r="F4">
+        <v>54.88</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5">
@@ -534,6 +540,12 @@
       </c>
       <c r="C5">
         <v>50</v>
+      </c>
+      <c r="D5">
+        <v>67.64</v>
+      </c>
+      <c r="F5">
+        <v>54.88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modified div and final_div parameters
</commit_message>
<xml_diff>
--- a/Observation.xlsx
+++ b/Observation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bala/Desktop/Projects/ERA/Session10/ModularRepository/modular/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C119AD0-055C-8F4E-BD52-EC83EDFB3C78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A610200-64A4-E941-910C-C724958DFD12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17180" xr2:uid="{F215A8E2-2D1F-A441-B7FA-652D74289773}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
   <si>
     <t>Parameter</t>
   </si>
@@ -430,10 +430,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14F4F4F4-6DB4-9E47-9C42-B8C813E0545D}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -527,8 +527,14 @@
       <c r="D4">
         <v>67.64</v>
       </c>
+      <c r="E4">
+        <v>86.45</v>
+      </c>
       <c r="F4">
         <v>54.88</v>
+      </c>
+      <c r="G4">
+        <v>86.25</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -544,8 +550,36 @@
       <c r="D5">
         <v>67.64</v>
       </c>
+      <c r="E5">
+        <v>86.45</v>
+      </c>
       <c r="F5">
         <v>54.88</v>
+      </c>
+      <c r="G5">
+        <v>86.25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>3</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>3</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="1">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added scheduler.step and modified params
</commit_message>
<xml_diff>
--- a/Observation.xlsx
+++ b/Observation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bala/Desktop/Projects/ERA/Session10/ModularRepository/modular/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A610200-64A4-E941-910C-C724958DFD12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F619B78C-20FA-E64B-8FF7-0830C11B8BA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17180" xr2:uid="{F215A8E2-2D1F-A441-B7FA-652D74289773}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="9">
   <si>
     <t>Parameter</t>
   </si>
@@ -86,7 +86,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -96,6 +96,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -112,10 +118,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -430,10 +437,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14F4F4F4-6DB4-9E47-9C42-B8C813E0545D}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -570,6 +577,18 @@
       <c r="C6" s="1">
         <v>1</v>
       </c>
+      <c r="D6" s="1">
+        <v>47.39</v>
+      </c>
+      <c r="E6" s="1">
+        <v>71.41</v>
+      </c>
+      <c r="F6" s="1">
+        <v>40.43</v>
+      </c>
+      <c r="G6" s="1">
+        <v>72.59</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
@@ -580,6 +599,178 @@
       </c>
       <c r="C7" s="1">
         <v>25</v>
+      </c>
+      <c r="D7" s="1">
+        <v>47.39</v>
+      </c>
+      <c r="E7" s="1">
+        <v>71.41</v>
+      </c>
+      <c r="F7" s="1">
+        <v>40.43</v>
+      </c>
+      <c r="G7" s="1">
+        <v>72.59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8">
+        <v>100</v>
+      </c>
+      <c r="D8">
+        <v>68.48</v>
+      </c>
+      <c r="E8">
+        <v>86.98</v>
+      </c>
+      <c r="F8">
+        <v>46.47</v>
+      </c>
+      <c r="G8">
+        <v>86.85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>4</v>
+      </c>
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9">
+        <v>100</v>
+      </c>
+      <c r="D9">
+        <v>68.48</v>
+      </c>
+      <c r="E9">
+        <v>86.98</v>
+      </c>
+      <c r="F9">
+        <v>46.47</v>
+      </c>
+      <c r="G9">
+        <v>86.85</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>5</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="1">
+        <v>500</v>
+      </c>
+      <c r="D10" s="1">
+        <v>68.09</v>
+      </c>
+      <c r="E10" s="1">
+        <v>86.76</v>
+      </c>
+      <c r="F10" s="1">
+        <v>57.65</v>
+      </c>
+      <c r="G10" s="1">
+        <v>86.2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>5</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="1">
+        <v>500</v>
+      </c>
+      <c r="D11" s="1">
+        <v>68.09</v>
+      </c>
+      <c r="E11" s="1">
+        <v>86.76</v>
+      </c>
+      <c r="F11" s="1">
+        <v>57.65</v>
+      </c>
+      <c r="G11" s="1">
+        <v>86.2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>6</v>
+      </c>
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12">
+        <v>100</v>
+      </c>
+      <c r="D12">
+        <v>68.260000000000005</v>
+      </c>
+      <c r="E12">
+        <v>87.12</v>
+      </c>
+      <c r="F12">
+        <v>30.35</v>
+      </c>
+      <c r="G12">
+        <v>86.74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>6</v>
+      </c>
+      <c r="B13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13">
+        <v>500</v>
+      </c>
+      <c r="D13">
+        <v>68.260000000000005</v>
+      </c>
+      <c r="E13">
+        <v>87.12</v>
+      </c>
+      <c r="F13">
+        <v>30.35</v>
+      </c>
+      <c r="G13">
+        <v>86.74</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="3">
+        <v>5</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="3">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="3">
+        <v>5</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="3">
+        <v>10000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
removed the scheduler.step() present inside the for loop in the training module
</commit_message>
<xml_diff>
--- a/Observation.xlsx
+++ b/Observation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bala/Desktop/Projects/ERA/Session10/ModularRepository/modular/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F619B78C-20FA-E64B-8FF7-0830C11B8BA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A625FEAD-317A-7B40-8A46-32B2E3394503}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17180" xr2:uid="{F215A8E2-2D1F-A441-B7FA-652D74289773}"/>
   </bookViews>
@@ -440,7 +440,7 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
observed new factor values
</commit_message>
<xml_diff>
--- a/Observation.xlsx
+++ b/Observation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bala/Desktop/Projects/ERA/Session10/ModularRepository/modular/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A625FEAD-317A-7B40-8A46-32B2E3394503}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0F61A61-8977-8445-BA7F-395070C00E42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17180" xr2:uid="{F215A8E2-2D1F-A441-B7FA-652D74289773}"/>
   </bookViews>
@@ -86,7 +86,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -96,12 +96,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -118,11 +112,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -440,15 +433,15 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.83203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -466,10 +459,10 @@
         <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>3</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>4</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>5</v>
@@ -489,10 +482,10 @@
         <v>67.88</v>
       </c>
       <c r="E2" s="1">
+        <v>49.52</v>
+      </c>
+      <c r="F2" s="1">
         <v>86.93</v>
-      </c>
-      <c r="F2" s="1">
-        <v>49.52</v>
       </c>
       <c r="G2" s="1">
         <v>86.46</v>
@@ -512,10 +505,10 @@
         <v>67.88</v>
       </c>
       <c r="E3" s="1">
+        <v>49.52</v>
+      </c>
+      <c r="F3" s="1">
         <v>86.93</v>
-      </c>
-      <c r="F3" s="1">
-        <v>49.52</v>
       </c>
       <c r="G3" s="1">
         <v>86.46</v>
@@ -535,10 +528,10 @@
         <v>67.64</v>
       </c>
       <c r="E4">
+        <v>54.88</v>
+      </c>
+      <c r="F4">
         <v>86.45</v>
-      </c>
-      <c r="F4">
-        <v>54.88</v>
       </c>
       <c r="G4">
         <v>86.25</v>
@@ -558,10 +551,10 @@
         <v>67.64</v>
       </c>
       <c r="E5">
+        <v>54.88</v>
+      </c>
+      <c r="F5">
         <v>86.45</v>
-      </c>
-      <c r="F5">
-        <v>54.88</v>
       </c>
       <c r="G5">
         <v>86.25</v>
@@ -581,10 +574,10 @@
         <v>47.39</v>
       </c>
       <c r="E6" s="1">
+        <v>40.43</v>
+      </c>
+      <c r="F6" s="1">
         <v>71.41</v>
-      </c>
-      <c r="F6" s="1">
-        <v>40.43</v>
       </c>
       <c r="G6" s="1">
         <v>72.59</v>
@@ -604,10 +597,10 @@
         <v>47.39</v>
       </c>
       <c r="E7" s="1">
+        <v>40.43</v>
+      </c>
+      <c r="F7" s="1">
         <v>71.41</v>
-      </c>
-      <c r="F7" s="1">
-        <v>40.43</v>
       </c>
       <c r="G7" s="1">
         <v>72.59</v>
@@ -627,10 +620,10 @@
         <v>68.48</v>
       </c>
       <c r="E8">
+        <v>46.47</v>
+      </c>
+      <c r="F8">
         <v>86.98</v>
-      </c>
-      <c r="F8">
-        <v>46.47</v>
       </c>
       <c r="G8">
         <v>86.85</v>
@@ -650,10 +643,10 @@
         <v>68.48</v>
       </c>
       <c r="E9">
+        <v>46.47</v>
+      </c>
+      <c r="F9">
         <v>86.98</v>
-      </c>
-      <c r="F9">
-        <v>46.47</v>
       </c>
       <c r="G9">
         <v>86.85</v>
@@ -673,10 +666,10 @@
         <v>68.09</v>
       </c>
       <c r="E10" s="1">
+        <v>57.65</v>
+      </c>
+      <c r="F10" s="1">
         <v>86.76</v>
-      </c>
-      <c r="F10" s="1">
-        <v>57.65</v>
       </c>
       <c r="G10" s="1">
         <v>86.2</v>
@@ -696,10 +689,10 @@
         <v>68.09</v>
       </c>
       <c r="E11" s="1">
+        <v>57.65</v>
+      </c>
+      <c r="F11" s="1">
         <v>86.76</v>
-      </c>
-      <c r="F11" s="1">
-        <v>57.65</v>
       </c>
       <c r="G11" s="1">
         <v>86.2</v>
@@ -719,10 +712,10 @@
         <v>68.260000000000005</v>
       </c>
       <c r="E12">
+        <v>30.35</v>
+      </c>
+      <c r="F12">
         <v>87.12</v>
-      </c>
-      <c r="F12">
-        <v>30.35</v>
       </c>
       <c r="G12">
         <v>86.74</v>
@@ -742,35 +735,59 @@
         <v>68.260000000000005</v>
       </c>
       <c r="E13">
+        <v>30.35</v>
+      </c>
+      <c r="F13">
         <v>87.12</v>
-      </c>
-      <c r="F13">
-        <v>30.35</v>
       </c>
       <c r="G13">
         <v>86.74</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="3">
-        <v>5</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14" s="3">
-        <v>10000</v>
+      <c r="A14" s="1">
+        <v>7</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="1">
+        <v>100</v>
+      </c>
+      <c r="D14">
+        <v>77.83</v>
+      </c>
+      <c r="E14">
+        <v>72.55</v>
+      </c>
+      <c r="F14">
+        <v>91.72</v>
+      </c>
+      <c r="G14">
+        <v>84.45</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="3">
-        <v>5</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C15" s="3">
-        <v>10000</v>
+      <c r="A15" s="1">
+        <v>7</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="1">
+        <v>100</v>
+      </c>
+      <c r="D15">
+        <v>77.83</v>
+      </c>
+      <c r="E15">
+        <v>72.55</v>
+      </c>
+      <c r="F15">
+        <v>91.72</v>
+      </c>
+      <c r="G15">
+        <v>84.45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
final_div_factor is set to None
</commit_message>
<xml_diff>
--- a/Observation.xlsx
+++ b/Observation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bala/Desktop/Projects/ERA/Session10/ModularRepository/modular/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D4065DD-CB2F-E046-A8E8-42E396BEDA80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AD9EB5D-DFAA-424C-A0CA-0E3E316ED775}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="14">
   <si>
     <t>Change_ID</t>
   </si>
@@ -65,12 +65,15 @@
   <si>
     <t>after every batch</t>
   </si>
+  <si>
+    <t>None</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -85,24 +88,34 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -113,6 +126,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -135,18 +154,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -365,7 +388,7 @@
   <dimension ref="A1:G1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -689,16 +712,16 @@
       <c r="C14" s="2">
         <v>100</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14" s="6">
         <v>77.83</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E14" s="6">
         <v>72.55</v>
       </c>
-      <c r="F14" s="3">
+      <c r="F14" s="6">
         <v>91.72</v>
       </c>
-      <c r="G14" s="3">
+      <c r="G14" s="6">
         <v>84.45</v>
       </c>
     </row>
@@ -712,16 +735,16 @@
       <c r="C15" s="2">
         <v>100</v>
       </c>
-      <c r="D15" s="3">
+      <c r="D15" s="6">
         <v>77.83</v>
       </c>
-      <c r="E15" s="3">
+      <c r="E15" s="6">
         <v>72.55</v>
       </c>
-      <c r="F15" s="3">
+      <c r="F15" s="6">
         <v>91.72</v>
       </c>
-      <c r="G15" s="3">
+      <c r="G15" s="6">
         <v>84.45</v>
       </c>
     </row>
@@ -748,32 +771,54 @@
         <v>85.7</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="5">
+    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="7">
         <v>9</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="7" t="s">
         <v>12</v>
       </c>
+      <c r="D17" s="9">
+        <v>70.040000000000006</v>
+      </c>
+      <c r="E17" s="9">
+        <v>43.51</v>
+      </c>
+      <c r="F17" s="10">
+        <v>89.94</v>
+      </c>
+      <c r="G17" s="10">
+        <v>88.33</v>
+      </c>
     </row>
-    <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="19" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="21" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="22" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="23" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="25" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>10</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
configured pct_start to 0.3 in params.yaml
</commit_message>
<xml_diff>
--- a/Observation.xlsx
+++ b/Observation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bala/Desktop/Projects/ERA/Session10/ModularRepository/modular/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AA0A589-C624-E44B-97F3-34A3D71959A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97B39EE7-1A54-1444-ADFA-4D3BF1527143}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="20">
   <si>
     <t>Change_ID</t>
   </si>
@@ -83,16 +83,26 @@
   <si>
     <t>10/EPOCHS</t>
   </si>
+  <si>
+    <t>23rd Epoch - ValueError: Tried to step 2353 times. The specified number of total steps is 2352</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -151,7 +161,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -167,6 +177,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -190,38 +212,40 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -440,7 +464,7 @@
   <dimension ref="A1:G1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -755,48 +779,48 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="2">
+      <c r="A14" s="17">
         <v>7</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="17">
         <v>100</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="18">
         <v>77.83</v>
       </c>
-      <c r="E14" s="5">
+      <c r="E14" s="18">
         <v>72.55</v>
       </c>
-      <c r="F14" s="5">
+      <c r="F14" s="18">
         <v>91.72</v>
       </c>
-      <c r="G14" s="5">
+      <c r="G14" s="18">
         <v>84.45</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="2">
+      <c r="A15" s="17">
         <v>7</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="17">
         <v>100</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D15" s="18">
         <v>77.83</v>
       </c>
-      <c r="E15" s="5">
+      <c r="E15" s="18">
         <v>72.55</v>
       </c>
-      <c r="F15" s="5">
+      <c r="F15" s="18">
         <v>91.72</v>
       </c>
-      <c r="G15" s="5">
+      <c r="G15" s="18">
         <v>84.45</v>
       </c>
     </row>
@@ -824,62 +848,62 @@
       </c>
     </row>
     <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="6">
+      <c r="A17" s="5">
         <v>9</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="15" t="s">
+      <c r="C17" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D17" s="8">
+      <c r="D17" s="7">
         <v>70.040000000000006</v>
       </c>
-      <c r="E17" s="8">
+      <c r="E17" s="7">
         <v>43.51</v>
       </c>
-      <c r="F17" s="9">
+      <c r="F17" s="8">
         <v>89.94</v>
       </c>
-      <c r="G17" s="9">
+      <c r="G17" s="8">
         <v>88.33</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="10">
+      <c r="A18" s="9">
         <v>10</v>
       </c>
-      <c r="B18" s="10" t="s">
+      <c r="B18" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C18" s="16" t="s">
+      <c r="C18" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="D18" s="10" t="s">
+      <c r="D18" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
     </row>
     <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="9">
+      <c r="A19" s="8">
         <v>11</v>
       </c>
-      <c r="B19" s="13" t="s">
+      <c r="B19" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="17" t="s">
+      <c r="C19" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="D19" s="11">
+      <c r="D19" s="10">
         <v>69.61</v>
       </c>
-      <c r="E19" s="11">
+      <c r="E19" s="10">
         <v>47.87</v>
       </c>
-      <c r="F19" s="14" t="s">
+      <c r="F19" s="12" t="s">
         <v>17</v>
       </c>
     </row>
@@ -887,15 +911,37 @@
       <c r="A20">
         <v>12</v>
       </c>
-      <c r="B20" s="12" t="s">
+      <c r="B20" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="C20" s="18" t="s">
+      <c r="C20" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="F20" s="12"/>
-    </row>
-    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="D20">
+        <v>72.430000000000007</v>
+      </c>
+      <c r="E20">
+        <v>55.25</v>
+      </c>
+      <c r="F20" s="19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="8">
+        <v>13</v>
+      </c>
+      <c r="B21" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="8">
+        <v>0.3</v>
+      </c>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+    </row>
     <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
reset pct_start, modified scheduler.step()
</commit_message>
<xml_diff>
--- a/Observation.xlsx
+++ b/Observation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bala/Desktop/Projects/ERA/Session10/ModularRepository/modular/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97B39EE7-1A54-1444-ADFA-4D3BF1527143}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBAE8FB2-59FD-7B4E-8D23-41B1E035091F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="21">
   <si>
     <t>Change_ID</t>
   </si>
@@ -85,17 +85,27 @@
   </si>
   <si>
     <t>23rd Epoch - ValueError: Tried to step 2353 times. The specified number of total steps is 2352</t>
+  </si>
+  <si>
+    <t>scheduler.step(sum(losses)/len(losses))</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -212,40 +222,44 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -464,7 +478,7 @@
   <dimension ref="A1:G1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -937,12 +951,30 @@
       <c r="C21" s="8">
         <v>0.3</v>
       </c>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
-    </row>
-    <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="D21" s="8">
+        <v>69.62</v>
+      </c>
+      <c r="E21" s="8">
+        <v>53.59</v>
+      </c>
+      <c r="F21" s="8">
+        <v>87.67</v>
+      </c>
+      <c r="G21" s="8">
+        <v>87.04</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>14</v>
+      </c>
+      <c r="B22" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" s="22" t="s">
+        <v>20</v>
+      </c>
+    </row>
     <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
added params for optimizers
</commit_message>
<xml_diff>
--- a/Observation.xlsx
+++ b/Observation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bala/Desktop/Projects/ERA/Session10/ModularRepository/modular/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBAE8FB2-59FD-7B4E-8D23-41B1E035091F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8233CC4-7649-5B42-BA74-D06A4A5F7FD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -222,7 +222,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -259,6 +259,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -478,7 +481,7 @@
   <dimension ref="A1:G1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -974,8 +977,24 @@
       <c r="C22" s="22" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="D22" s="23">
+        <v>78.06</v>
+      </c>
+      <c r="E22" s="23">
+        <v>75.180000000000007</v>
+      </c>
+      <c r="F22">
+        <v>91.37</v>
+      </c>
+      <c r="G22">
+        <v>84.65</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>15</v>
+      </c>
+    </row>
     <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
modified params in optimizer weight-decay
</commit_message>
<xml_diff>
--- a/Observation.xlsx
+++ b/Observation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bala/Desktop/Projects/ERA/Session10/ModularRepository/modular/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8233CC4-7649-5B42-BA74-D06A4A5F7FD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69510A1E-9B7A-B44D-842B-3589D2EE2132}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="23">
   <si>
     <t>Change_ID</t>
   </si>
@@ -88,17 +88,30 @@
   </si>
   <si>
     <t>scheduler.step(sum(losses)/len(losses))</t>
+  </si>
+  <si>
+    <t>optimizer - weight decay</t>
+  </si>
+  <si>
+    <t>optimizer_learning_rate</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -222,47 +235,48 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -481,14 +495,14 @@
   <dimension ref="A1:G1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.5" customWidth="1"/>
-    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24.6640625" customWidth="1"/>
     <col min="5" max="5" width="24" customWidth="1"/>
     <col min="6" max="6" width="16.83203125" customWidth="1"/>
@@ -991,12 +1005,62 @@
       </c>
     </row>
     <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23">
+      <c r="A23" s="12">
         <v>15</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="B23" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" s="12">
+        <v>0.9</v>
+      </c>
+      <c r="D23" s="12">
+        <v>56.29</v>
+      </c>
+      <c r="E23" s="12">
+        <v>38.82</v>
+      </c>
+      <c r="F23" s="12">
+        <v>51.26</v>
+      </c>
+      <c r="G23" s="12">
+        <v>37.68</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="12">
+        <v>15</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C24" s="12">
+        <v>0.03</v>
+      </c>
+      <c r="D24" s="12">
+        <v>56.29</v>
+      </c>
+      <c r="E24" s="12">
+        <v>38.82</v>
+      </c>
+      <c r="F24" s="12">
+        <v>51.26</v>
+      </c>
+      <c r="G24" s="12">
+        <v>37.68</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>16</v>
+      </c>
+      <c r="B25" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+    </row>
     <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
weight decay modidifed, added .gitignore
</commit_message>
<xml_diff>
--- a/Observation.xlsx
+++ b/Observation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bala/Desktop/Projects/ERA/Session10/ModularRepository/modular/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28D13415-8CB6-5640-845B-E548A298B3A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDEF6E81-F31A-BB45-8176-B8BF9A2A34D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="23">
   <si>
     <t>Change_ID</t>
   </si>
@@ -495,7 +495,7 @@
   <dimension ref="A1:G1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1060,8 +1060,24 @@
       <c r="C25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="D25">
+        <v>78.16</v>
+      </c>
+      <c r="E25">
+        <v>68.510000000000005</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>17</v>
+      </c>
+      <c r="B26" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="C26">
+        <v>1E-3</v>
+      </c>
+    </row>
     <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="29" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
param optimizer weight decay
</commit_message>
<xml_diff>
--- a/Observation.xlsx
+++ b/Observation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bala/Desktop/Projects/ERA/Session10/ModularRepository/modular/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDEF6E81-F31A-BB45-8176-B8BF9A2A34D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C22AE686-4143-C44A-ADA3-A6D263599A26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="23">
   <si>
     <t>Change_ID</t>
   </si>
@@ -100,11 +100,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -235,45 +242,46 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -495,7 +503,7 @@
   <dimension ref="A1:G1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -810,131 +818,131 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="17">
+      <c r="A14" s="16">
         <v>7</v>
       </c>
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="17">
+      <c r="C14" s="16">
         <v>100</v>
       </c>
-      <c r="D14" s="18">
+      <c r="D14" s="17">
         <v>77.83</v>
       </c>
-      <c r="E14" s="18">
+      <c r="E14" s="17">
         <v>72.55</v>
       </c>
-      <c r="F14" s="18">
+      <c r="F14" s="17">
         <v>91.72</v>
       </c>
-      <c r="G14" s="18">
+      <c r="G14" s="17">
         <v>84.45</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="17">
+      <c r="A15" s="16">
         <v>7</v>
       </c>
-      <c r="B15" s="17" t="s">
+      <c r="B15" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="17">
+      <c r="C15" s="16">
         <v>100</v>
       </c>
-      <c r="D15" s="18">
+      <c r="D15" s="17">
         <v>77.83</v>
       </c>
-      <c r="E15" s="18">
+      <c r="E15" s="17">
         <v>72.55</v>
       </c>
-      <c r="F15" s="18">
+      <c r="F15" s="17">
         <v>91.72</v>
       </c>
-      <c r="G15" s="18">
+      <c r="G15" s="17">
         <v>84.45</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="3">
+      <c r="A16" s="17">
         <v>8</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="D16" s="3">
+      <c r="D16" s="17">
         <v>78.28</v>
       </c>
-      <c r="E16" s="3">
+      <c r="E16" s="17">
         <v>73.73</v>
       </c>
-      <c r="F16" s="3">
+      <c r="F16" s="17">
         <v>91.53</v>
       </c>
-      <c r="G16" s="3">
+      <c r="G16" s="17">
         <v>85.7</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="5">
+      <c r="A17" s="4">
         <v>9</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="C17" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="D17" s="7">
+      <c r="D17" s="6">
         <v>70.040000000000006</v>
       </c>
-      <c r="E17" s="7">
+      <c r="E17" s="6">
         <v>43.51</v>
       </c>
-      <c r="F17" s="8">
+      <c r="F17" s="7">
         <v>89.94</v>
       </c>
-      <c r="G17" s="8">
+      <c r="G17" s="7">
         <v>88.33</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="9">
+      <c r="A18" s="8">
         <v>10</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="B18" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="C18" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="D18" s="9" t="s">
+      <c r="D18" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
     </row>
     <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="8">
+      <c r="A19" s="7">
         <v>11</v>
       </c>
-      <c r="B19" s="11" t="s">
+      <c r="B19" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="15" t="s">
+      <c r="C19" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="D19" s="10">
+      <c r="D19" s="9">
         <v>69.61</v>
       </c>
-      <c r="E19" s="10">
+      <c r="E19" s="9">
         <v>47.87</v>
       </c>
-      <c r="F19" s="12" t="s">
+      <c r="F19" s="11" t="s">
         <v>17</v>
       </c>
     </row>
@@ -942,10 +950,10 @@
       <c r="A20">
         <v>12</v>
       </c>
-      <c r="B20" s="19" t="s">
+      <c r="B20" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="C20" s="16" t="s">
+      <c r="C20" s="15" t="s">
         <v>18</v>
       </c>
       <c r="D20">
@@ -954,30 +962,30 @@
       <c r="E20">
         <v>55.25</v>
       </c>
-      <c r="F20" s="19" t="s">
+      <c r="F20" s="18" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="8">
+      <c r="A21" s="7">
         <v>13</v>
       </c>
-      <c r="B21" s="20" t="s">
+      <c r="B21" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="C21" s="8">
+      <c r="C21" s="7">
         <v>0.3</v>
       </c>
-      <c r="D21" s="8">
+      <c r="D21" s="7">
         <v>69.62</v>
       </c>
-      <c r="E21" s="8">
+      <c r="E21" s="7">
         <v>53.59</v>
       </c>
-      <c r="F21" s="8">
+      <c r="F21" s="7">
         <v>87.67</v>
       </c>
-      <c r="G21" s="8">
+      <c r="G21" s="7">
         <v>87.04</v>
       </c>
     </row>
@@ -985,16 +993,16 @@
       <c r="A22">
         <v>14</v>
       </c>
-      <c r="B22" s="21" t="s">
+      <c r="B22" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="C22" s="22" t="s">
+      <c r="C22" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="D22" s="23">
+      <c r="D22" s="22">
         <v>78.06</v>
       </c>
-      <c r="E22" s="23">
+      <c r="E22" s="22">
         <v>75.180000000000007</v>
       </c>
       <c r="F22">
@@ -1005,48 +1013,48 @@
       </c>
     </row>
     <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="12">
+      <c r="A23" s="11">
         <v>15</v>
       </c>
-      <c r="B23" s="12" t="s">
+      <c r="B23" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="12">
+      <c r="C23" s="11">
         <v>0.9</v>
       </c>
-      <c r="D23" s="12">
+      <c r="D23" s="11">
         <v>56.29</v>
       </c>
-      <c r="E23" s="12">
+      <c r="E23" s="11">
         <v>38.82</v>
       </c>
-      <c r="F23" s="12">
+      <c r="F23" s="11">
         <v>51.26</v>
       </c>
-      <c r="G23" s="12">
+      <c r="G23" s="11">
         <v>37.68</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="12">
+      <c r="A24" s="11">
         <v>15</v>
       </c>
-      <c r="B24" s="12" t="s">
+      <c r="B24" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C24" s="12">
+      <c r="C24" s="11">
         <v>0.03</v>
       </c>
-      <c r="D24" s="12">
+      <c r="D24" s="11">
         <v>56.29</v>
       </c>
-      <c r="E24" s="12">
+      <c r="E24" s="11">
         <v>38.82</v>
       </c>
-      <c r="F24" s="12">
+      <c r="F24" s="11">
         <v>51.26</v>
       </c>
-      <c r="G24" s="12">
+      <c r="G24" s="11">
         <v>37.68</v>
       </c>
     </row>
@@ -1054,7 +1062,7 @@
       <c r="A25">
         <v>16</v>
       </c>
-      <c r="B25" s="24" t="s">
+      <c r="B25" s="23" t="s">
         <v>21</v>
       </c>
       <c r="C25">
@@ -1065,20 +1073,36 @@
       </c>
       <c r="E25">
         <v>68.510000000000005</v>
+      </c>
+      <c r="F25">
+        <v>91.79</v>
+      </c>
+      <c r="G25">
+        <v>86.19</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>17</v>
       </c>
-      <c r="B26" s="24" t="s">
+      <c r="B26" s="23" t="s">
         <v>21</v>
       </c>
       <c r="C26">
         <v>1E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>18</v>
+      </c>
+      <c r="B27" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="C27">
+        <v>0.01</v>
+      </c>
+    </row>
     <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="29" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="30" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>